<commit_message>
Finished update feature including basic posting flow test from create, generate form, and update
</commit_message>
<xml_diff>
--- a/src/apodeixi/knowledge_base/tests_integration/input_data/basic_posting_flows/big_rocks.big-rocks.journeys.a6i.xlsx
+++ b/src/apodeixi/knowledge_base/tests_integration/input_data/basic_posting_flows/big_rocks.big-rocks.journeys.a6i.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\knowledge_base\tests_integration\input_data\basic_posting_flows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E56F064-37E8-4B72-930A-A8D652C0A623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F41D88-ECEA-43DB-B2A4-5F4AF4781D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Posting Label" sheetId="1" r:id="rId1"/>
@@ -187,9 +187,6 @@
     <t>Modernization – Persona Based Dashboard, Improved UI/UX</t>
   </si>
   <si>
-    <t>Services</t>
-  </si>
-  <si>
     <t>Containerization</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>F2:G8</t>
+  </si>
+  <si>
+    <t>Services (but for this v2, only the key ones)</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -872,7 +872,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
@@ -896,7 +896,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
@@ -920,7 +920,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -956,13 +956,13 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.45">
@@ -973,16 +973,16 @@
         <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="H2" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.45">
@@ -996,7 +996,7 @@
         <v>4050</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" s="7">
         <v>3584</v>
@@ -1017,7 +1017,7 @@
         <v>6600</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G4" s="7">
         <v>5207</v>
@@ -1038,7 +1038,7 @@
         <v>4500</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G5" s="7">
         <v>5575</v>
@@ -1053,13 +1053,13 @@
         <v>46</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="D6" s="7">
         <v>10351</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="7">
         <v>5800</v>
@@ -1072,13 +1072,13 @@
     <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="7">
         <v>999</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="7">
         <v>5860</v>
@@ -1093,13 +1093,13 @@
         <v>47</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="7">
         <v>525</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8" s="7">
         <v>999</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C9" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="8">
         <f>SUM(D3:D8)</f>

</xml_diff>